<commit_message>
Added total captures to report
</commit_message>
<xml_diff>
--- a/Assignment3/doc/results.xlsx
+++ b/Assignment3/doc/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>#Candidates</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>Max lvl</t>
+  </si>
+  <si>
+    <t>Tot cap</t>
   </si>
 </sst>
 </file>
@@ -354,11 +357,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75059200"/>
-        <c:axId val="59585280"/>
+        <c:axId val="92596096"/>
+        <c:axId val="92597632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75059200"/>
+        <c:axId val="92596096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -369,12 +372,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59585280"/>
+        <c:crossAx val="92597632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59585280"/>
+        <c:axId val="92597632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="130"/>
@@ -387,7 +390,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75059200"/>
+        <c:crossAx val="92596096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -543,11 +546,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75084544"/>
-        <c:axId val="75086080"/>
+        <c:axId val="92752896"/>
+        <c:axId val="92775168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75084544"/>
+        <c:axId val="92752896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -558,12 +561,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75086080"/>
+        <c:crossAx val="92775168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75086080"/>
+        <c:axId val="92775168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="900"/>
@@ -576,7 +579,175 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75084544"/>
+        <c:crossAx val="92752896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Total captures</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>655</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1470</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1357</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="49594752"/>
+        <c:axId val="49596288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="49594752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49596288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="49596288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1500"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49594752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -602,16 +773,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -632,16 +803,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -657,6 +828,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -952,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +1166,7 @@
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -973,8 +1176,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -984,8 +1190,11 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -995,8 +1204,11 @@
       <c r="C3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
@@ -1006,8 +1218,11 @@
       <c r="C4">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>30</v>
       </c>
@@ -1017,8 +1232,11 @@
       <c r="C5">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50</v>
       </c>
@@ -1028,8 +1246,11 @@
       <c r="C6">
         <v>190</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>80</v>
       </c>
@@ -1039,8 +1260,11 @@
       <c r="C7">
         <v>329</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>100</v>
       </c>
@@ -1050,8 +1274,11 @@
       <c r="C8">
         <v>427</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>130</v>
       </c>
@@ -1061,8 +1288,11 @@
       <c r="C9">
         <v>588</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>150</v>
       </c>
@@ -1072,49 +1302,52 @@
       <c r="C10">
         <v>654</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12">
-        <f>(A12*LN(A12)+A12)*0.1</f>
+        <f t="shared" ref="B12:B32" si="0">(A12*LN(A12)+A12)*0.1</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13">
-        <f>(A13*LN(A13)+A13)*0.1</f>
+        <f t="shared" si="0"/>
         <v>3.3025850929940463</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20</v>
       </c>
       <c r="B14">
-        <f>(A14*LN(A14)+A14)*0.1</f>
+        <f t="shared" si="0"/>
         <v>7.9914645471079808</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>30</v>
       </c>
       <c r="B15">
-        <f>(A15*LN(A15)+A15)*0.1</f>
+        <f t="shared" si="0"/>
         <v>13.203592144986466</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>40</v>
       </c>
       <c r="B16">
-        <f>(A16*LN(A16)+A16)*0.1</f>
+        <f t="shared" si="0"/>
         <v>18.755517816455747</v>
       </c>
     </row>
@@ -1123,7 +1356,7 @@
         <v>50</v>
       </c>
       <c r="B17">
-        <f>(A17*LN(A17)+A17)*0.1</f>
+        <f t="shared" si="0"/>
         <v>24.560115027140732</v>
       </c>
     </row>
@@ -1132,7 +1365,7 @@
         <v>60</v>
       </c>
       <c r="B18">
-        <f>(A18*LN(A18)+A18)*0.1</f>
+        <f t="shared" si="0"/>
         <v>30.566067373332601</v>
       </c>
     </row>
@@ -1141,7 +1374,7 @@
         <v>70</v>
       </c>
       <c r="B19">
-        <f>(A19*LN(A19)+A19)*0.1</f>
+        <f t="shared" si="0"/>
         <v>36.739466694345516</v>
       </c>
     </row>
@@ -1150,7 +1383,7 @@
         <v>80</v>
       </c>
       <c r="B20">
-        <f>(A20*LN(A20)+A20)*0.1</f>
+        <f t="shared" si="0"/>
         <v>43.05621307739105</v>
       </c>
     </row>
@@ -1159,7 +1392,7 @@
         <v>90</v>
       </c>
       <c r="B21">
-        <f>(A21*LN(A21)+A21)*0.1</f>
+        <f t="shared" si="0"/>
         <v>49.498287032972385</v>
       </c>
     </row>
@@ -1168,7 +1401,7 @@
         <v>100</v>
       </c>
       <c r="B22">
-        <f>(A22*LN(A22)+A22)*0.1</f>
+        <f t="shared" si="0"/>
         <v>56.051701859880922</v>
       </c>
     </row>
@@ -1177,7 +1410,7 @@
         <v>110</v>
       </c>
       <c r="B23">
-        <f>(A23*LN(A23)+A23)*0.1</f>
+        <f t="shared" si="0"/>
         <v>62.705284023716587</v>
       </c>
     </row>
@@ -1186,7 +1419,7 @@
         <v>120</v>
       </c>
       <c r="B24">
-        <f>(A24*LN(A24)+A24)*0.1</f>
+        <f t="shared" si="0"/>
         <v>69.449900913384553</v>
       </c>
     </row>
@@ -1195,7 +1428,7 @@
         <v>130</v>
       </c>
       <c r="B25">
-        <f>(A25*LN(A25)+A25)*0.1</f>
+        <f t="shared" si="0"/>
         <v>76.277947855922577</v>
       </c>
     </row>
@@ -1204,7 +1437,7 @@
         <v>140</v>
       </c>
       <c r="B26">
-        <f>(A26*LN(A26)+A26)*0.1</f>
+        <f t="shared" si="0"/>
         <v>83.182993916530265</v>
       </c>
     </row>
@@ -1213,7 +1446,7 @@
         <v>150</v>
       </c>
       <c r="B27">
-        <f>(A27*LN(A27)+A27)*0.1</f>
+        <f t="shared" si="0"/>
         <v>90.159529411443827</v>
       </c>
     </row>
@@ -1222,7 +1455,7 @@
         <v>160</v>
       </c>
       <c r="B28">
-        <f>(A28*LN(A28)+A28)*0.1</f>
+        <f t="shared" si="0"/>
         <v>97.202781043741226</v>
       </c>
     </row>
@@ -1231,7 +1464,7 @@
         <v>170</v>
       </c>
       <c r="B29">
-        <f>(A29*LN(A29)+A29)*0.1</f>
+        <f t="shared" si="0"/>
         <v>104.30857342985446</v>
       </c>
     </row>
@@ -1240,7 +1473,7 @@
         <v>180</v>
       </c>
       <c r="B30">
-        <f>(A30*LN(A30)+A30)*0.1</f>
+        <f t="shared" si="0"/>
         <v>111.47322331602379</v>
       </c>
     </row>
@@ -1249,7 +1482,7 @@
         <v>190</v>
       </c>
       <c r="B31">
-        <f>(A31*LN(A31)+A31)*0.1</f>
+        <f t="shared" si="0"/>
         <v>118.69345737104923</v>
       </c>
     </row>
@@ -1258,7 +1491,7 @@
         <v>200</v>
       </c>
       <c r="B32">
-        <f>(A32*LN(A32)+A32)*0.1</f>
+        <f t="shared" si="0"/>
         <v>125.96634733096073</v>
       </c>
     </row>

</xml_diff>